<commit_message>
Regular update #0714 💯
</commit_message>
<xml_diff>
--- a/public/download/download_sample.xlsx
+++ b/public/download/download_sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="2018年度XX月份地区销量测试表" sheetId="1" r:id="rId1"/>
+    <sheet name="876987" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -379,134 +379,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>省份</v>
+        <v>海南</v>
       </c>
       <c r="B1" t="str">
-        <v>销量</v>
+        <v/>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>广东</v>
+        <v>云南</v>
       </c>
       <c r="B2" t="str">
-        <v>1522</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>广西</v>
+        <v>贵州</v>
       </c>
       <c r="B3" t="str">
-        <v>677</v>
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>海南</v>
+        <v>湖南</v>
       </c>
       <c r="B4" t="str">
-        <v>389</v>
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>云南</v>
+        <v>江西</v>
       </c>
       <c r="B5" t="str">
-        <v>502</v>
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>贵州</v>
+        <v>北京</v>
       </c>
       <c r="B6" t="str">
-        <v>448</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>湖南</v>
+        <v>上海</v>
       </c>
       <c r="B7" t="str">
-        <v>1010</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>江西</v>
+        <v>江苏</v>
       </c>
       <c r="B8" t="str">
-        <v>490</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>北京</v>
+        <v>浙江</v>
       </c>
       <c r="B9" t="str">
-        <v>910</v>
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>上海</v>
+        <v>福建</v>
       </c>
       <c r="B10" t="str">
-        <v>654</v>
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>江苏</v>
+        <v>四川</v>
       </c>
       <c r="B11" t="str">
-        <v>309</v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>浙江</v>
+        <v>陕西</v>
       </c>
       <c r="B12" t="str">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>福建</v>
-      </c>
-      <c r="B13" t="str">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>四川</v>
-      </c>
-      <c r="B14" t="str">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>陕西</v>
-      </c>
-      <c r="B15" t="str">
-        <v>520</v>
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>